<commit_message>
refacter unmerge so now it freaking work flawleslly without to use unmerge agian, i nuke the merge starting from starting row
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/JLFHM.xlsx
+++ b/invoice_gen/TEMPLATE/JLFHM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\inv_pkl_contract_creation\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457DE0CE-3270-42A2-AD7F-34D05FDEAA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A14C78-E222-4548-B7FC-AACB9DEF4CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice!$A$1:$G$30</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Packing list'!$A$1:$I$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Packing list'!$A$1:$I$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1145,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -1399,140 +1399,160 @@
       <c r="B19" s="19"/>
     </row>
     <row r="20" spans="1:9" ht="27.75" customHeight="1">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-    </row>
-    <row r="21" spans="1:9" ht="42" customHeight="1">
-      <c r="A21" s="40" t="s">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" ht="27.75" customHeight="1">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+    </row>
+    <row r="22" spans="1:9" ht="27.75" customHeight="1">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" ht="27.75" customHeight="1">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+    </row>
+    <row r="24" spans="1:9" ht="27.75" customHeight="1">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+    </row>
+    <row r="25" spans="1:9" ht="27.75" customHeight="1">
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+    </row>
+    <row r="26" spans="1:9" ht="42" customHeight="1">
+      <c r="A26" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" ht="74.099999999999994" customHeight="1">
-      <c r="A22" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" ht="44.1" customHeight="1">
-      <c r="A23" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A24" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-    </row>
-    <row r="25" spans="1:9" s="1" customFormat="1" ht="27" customHeight="1">
-      <c r="A25" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-    </row>
-    <row r="26" spans="1:9" ht="42" customHeight="1">
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="9" t="s">
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" ht="74.099999999999994" customHeight="1">
+      <c r="A27" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="41"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" ht="44.1" customHeight="1">
+      <c r="A28" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A29" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+    </row>
+    <row r="30" spans="1:9" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="A30" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+    </row>
+    <row r="31" spans="1:9" ht="42" customHeight="1">
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" ht="24" customHeight="1">
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="29"/>
-    </row>
-    <row r="28" spans="1:9" ht="69.75" customHeight="1">
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" ht="42" customHeight="1">
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" ht="53.1" customHeight="1">
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" ht="27.75" customHeight="1"/>
-    <row r="32" spans="1:9" ht="27.75" customHeight="1"/>
-    <row r="33" ht="27.75" customHeight="1"/>
-    <row r="34" ht="24.75" customHeight="1"/>
-    <row r="35" ht="21" customHeight="1"/>
-    <row r="36" ht="21" customHeight="1"/>
-    <row r="37" ht="21" customHeight="1"/>
-    <row r="38" ht="21" customHeight="1"/>
-    <row r="39" ht="21" customHeight="1"/>
-    <row r="40" ht="21" customHeight="1"/>
-    <row r="41" ht="21" customHeight="1"/>
-    <row r="42" ht="21" customHeight="1"/>
-    <row r="43" ht="25.5" customHeight="1"/>
-    <row r="44" ht="21" customHeight="1"/>
-    <row r="45" ht="21" customHeight="1"/>
-    <row r="46" ht="21" customHeight="1"/>
-    <row r="47" ht="21" customHeight="1"/>
-    <row r="48" ht="21" customHeight="1"/>
-    <row r="49" ht="17.25" customHeight="1"/>
-    <row r="61" ht="15" customHeight="1"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" ht="24" customHeight="1">
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="29"/>
+    </row>
+    <row r="33" spans="6:9" ht="69.75" customHeight="1">
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="6:9" ht="42" customHeight="1">
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="6:9" ht="53.1" customHeight="1">
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="6:9" ht="27.75" customHeight="1"/>
+    <row r="37" spans="6:9" ht="27.75" customHeight="1"/>
+    <row r="38" spans="6:9" ht="27.75" customHeight="1"/>
+    <row r="39" spans="6:9" ht="24.75" customHeight="1"/>
+    <row r="40" spans="6:9" ht="21" customHeight="1"/>
+    <row r="41" spans="6:9" ht="21" customHeight="1"/>
+    <row r="42" spans="6:9" ht="21" customHeight="1"/>
+    <row r="43" spans="6:9" ht="21" customHeight="1"/>
+    <row r="44" spans="6:9" ht="21" customHeight="1"/>
+    <row r="45" spans="6:9" ht="21" customHeight="1"/>
+    <row r="46" spans="6:9" ht="21" customHeight="1"/>
+    <row r="47" spans="6:9" ht="21" customHeight="1"/>
+    <row r="48" spans="6:9" ht="25.5" customHeight="1"/>
+    <row r="49" ht="21" customHeight="1"/>
+    <row r="50" ht="21" customHeight="1"/>
+    <row r="51" ht="21" customHeight="1"/>
+    <row r="52" ht="21" customHeight="1"/>
+    <row r="53" ht="21" customHeight="1"/>
+    <row r="54" ht="17.25" customHeight="1"/>
+    <row r="66" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A25:I25"/>
+    <mergeCell ref="A30:I30"/>
     <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:I29"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>

</xml_diff>